<commit_message>
v2.1.1 update: Restructured AI stats. - All AI profiles simplified and added to metrics. - Renamed Infiltrate to Infiltrator. - Renamed Marching Order to Commanding Presence. - Renamed Cowardly to Cautious. - Fixed typo in Shredding rule. - Clarified Infiltrator rule description. - Updated rulebook.
</commit_message>
<xml_diff>
--- a/metrics/XCOM Enemy Eternal - Costs and Statistics.xlsx
+++ b/metrics/XCOM Enemy Eternal - Costs and Statistics.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phoenix\source\repos\KabelKabal\BardIndex\Eklipse Games\XCOM Enemy Eternal\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phoenix\source\repos\Eklipse-Games\xcom-enemyeternal\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9D9BB4-177B-4CBF-B2E7-B239A44D7A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CA7162-B142-4F52-9455-11B9C15E8CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EB47B550-E58A-4646-B89E-9CBA77073B0E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EB47B550-E58A-4646-B89E-9CBA77073B0E}"/>
   </bookViews>
   <sheets>
     <sheet name="UNIT STATS" sheetId="1" r:id="rId1"/>
+    <sheet name="AI STATS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UNIT STATS'!$A$3:$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'AI STATS'!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UNIT STATS'!$A$3:$N$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
-  <si>
-    <t>XCOM Rookie</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
   <si>
     <t>AIM</t>
   </si>
@@ -68,18 +67,6 @@
     <t>Special Rules</t>
   </si>
   <si>
-    <t>XCOM Specialist</t>
-  </si>
-  <si>
-    <t>XCOM Ranger</t>
-  </si>
-  <si>
-    <t>XCOM Grenadier</t>
-  </si>
-  <si>
-    <t>XCOM Sharpshooter</t>
-  </si>
-  <si>
     <t>UNIT NAME</t>
   </si>
   <si>
@@ -89,9 +76,6 @@
     <t>PSI</t>
   </si>
   <si>
-    <t>/-</t>
-  </si>
-  <si>
     <t>ADVENT Trooper</t>
   </si>
   <si>
@@ -149,21 +133,12 @@
     <t>Viper</t>
   </si>
   <si>
-    <t>Rules</t>
-  </si>
-  <si>
     <t>Phantom</t>
   </si>
   <si>
     <t>Squad Tactics, Weak Minded</t>
   </si>
   <si>
-    <t>Infiltrate, Weak Minded</t>
-  </si>
-  <si>
-    <t>Marching Order</t>
-  </si>
-  <si>
     <t>Unstable</t>
   </si>
   <si>
@@ -182,20 +157,235 @@
     <t>Deadeye</t>
   </si>
   <si>
-    <t>Cowardly</t>
+    <t>Infiltrator, Weak Minded</t>
+  </si>
+  <si>
+    <t>Commanding Presence</t>
+  </si>
+  <si>
+    <t>Cautious</t>
+  </si>
+  <si>
+    <t>AI STATS</t>
+  </si>
+  <si>
+    <t>Priorities</t>
+  </si>
+  <si>
+    <t>Grenadier</t>
+  </si>
+  <si>
+    <t>Rookie</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Specialist</t>
+  </si>
+  <si>
+    <t>Sharpshooter</t>
+  </si>
+  <si>
+    <t>Will never take cover.
+1. Closest
+2. Strongest
+3. Wounded</t>
+  </si>
+  <si>
+    <t>A!* (3+)
+A!* (1-2)</t>
+  </si>
+  <si>
+    <t>O!* (3+)
+M!* (1-2)</t>
+  </si>
+  <si>
+    <t>O!* (3+)
+A! (1-2)</t>
+  </si>
+  <si>
+    <t>1 - Omega</t>
+  </si>
+  <si>
+    <t>2-3 - Delta</t>
+  </si>
+  <si>
+    <t>4-5 - Bravo</t>
+  </si>
+  <si>
+    <t>6 - Alpha</t>
+  </si>
+  <si>
+    <t>O! (3+)
+D! (1-2)</t>
+  </si>
+  <si>
+    <t>O! (3+)
+O* (1-2)</t>
+  </si>
+  <si>
+    <t>A! (3+)
+A* (1-2)</t>
+  </si>
+  <si>
+    <t>A! (3+)
+A!* (1-2)</t>
+  </si>
+  <si>
+    <t>1. Strongest
+2. Closest
+3. Healthiest</t>
+  </si>
+  <si>
+    <t>A! (3+)
+F!* (1-2)</t>
+  </si>
+  <si>
+    <t>O (3+)
+F (1-2)</t>
+  </si>
+  <si>
+    <t>A (3+)
+M! (1-2)</t>
+  </si>
+  <si>
+    <t>A! (3+)
+A (1-2)</t>
+  </si>
+  <si>
+    <t>[Mindspin] preference.
+1. Wounded
+2. Weakest
+3. Closest</t>
+  </si>
+  <si>
+    <t>M (3+)
+D (1-2)</t>
+  </si>
+  <si>
+    <t>A (3+)
+A! (1-2)</t>
+  </si>
+  <si>
+    <t>A (3+)
+D (1-2)</t>
+  </si>
+  <si>
+    <t>A (3+)
+A (1-2)</t>
+  </si>
+  <si>
+    <t>1. Furthest
+2. Wounded
+3. Weakest</t>
+  </si>
+  <si>
+    <t>D (3+)
+F! (1-2)</t>
+  </si>
+  <si>
+    <t>D! (3+)
+D! (1-2)</t>
+  </si>
+  <si>
+    <t>D (3+)
+D! (1-2)</t>
+  </si>
+  <si>
+    <t>A (3+)
+F (1-2)</t>
+  </si>
+  <si>
+    <t>Special Rules preference.
+1. Wounded
+2. Weakest
+3. Closest</t>
+  </si>
+  <si>
+    <t>A! (3+)
+D! (1-2)</t>
+  </si>
+  <si>
+    <t>O (3+)
+A! (1-2)</t>
+  </si>
+  <si>
+    <t>O! (3+)
+M! (1-2)</t>
+  </si>
+  <si>
+    <t>O! (3+)
+O!* (1-2)</t>
+  </si>
+  <si>
+    <t>[Secondary Weapon] preference.
+1. Closest
+2. Weakest
+3. Wounded</t>
+  </si>
+  <si>
+    <t>F (3+)
+F! (1-2)</t>
+  </si>
+  <si>
+    <t>O (3+)
+O (1-2)</t>
+  </si>
+  <si>
+    <t>A (3+)
+M (1-2)</t>
+  </si>
+  <si>
+    <t>1. Wounded
+2. Closest
+3. Strongest</t>
+  </si>
+  <si>
+    <t>Faceless (AI)</t>
+  </si>
+  <si>
+    <t>Heavy-Focused (AI)</t>
+  </si>
+  <si>
+    <t>Psi-Focused (AI)</t>
+  </si>
+  <si>
+    <t>Sniper-Focused (AI)</t>
+  </si>
+  <si>
+    <t>Support-Focused (AI)</t>
+  </si>
+  <si>
+    <t>Tackler-Focused (AI)</t>
+  </si>
+  <si>
+    <t>Trooper-Focused (AI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,10 +423,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,17 +772,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63DEB86-B494-49C7-AE29-DB56967CB25B}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
@@ -589,72 +790,68 @@
     <col min="9" max="9" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.26953125" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -680,30 +877,27 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4">
+      <c r="L4">
         <f>D4+E4+F4+G4+H4+I4+J4+K4</f>
         <v>34</v>
       </c>
-      <c r="N4">
-        <f>M4*3</f>
+      <c r="M4">
+        <f>L4*3</f>
         <v>102</v>
       </c>
-      <c r="O4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -729,30 +923,27 @@
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5">
+      <c r="L5">
         <f>D5+E5+F5+G5+H5+I5+J5+K5</f>
         <v>35</v>
       </c>
-      <c r="N5">
-        <f>M5*3</f>
+      <c r="M5">
+        <f>L5*3</f>
         <v>105</v>
       </c>
-      <c r="O5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -778,94 +969,88 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6">
+      <c r="L6">
         <f>D6+E6+F6+G6+H6+I6+J6+K6</f>
         <v>34</v>
       </c>
-      <c r="N6">
-        <f>M6*3</f>
+      <c r="M6">
+        <f>L6*3</f>
         <v>102</v>
       </c>
-      <c r="O6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
         <v>8</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
-        <v>16</v>
+      <c r="L7">
+        <f>D7+E7+F7+G7+H7+I7+J7+K7</f>
+        <v>35</v>
       </c>
       <c r="M7">
-        <f>D7+E7+F7+G7+H7+I7+J7+K7</f>
-        <v>34</v>
-      </c>
-      <c r="N7">
-        <f>M7*3</f>
-        <v>102</v>
-      </c>
-      <c r="O7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+        <f>L7*3</f>
+        <v>105</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8">
         <v>3</v>
@@ -876,128 +1061,119 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
-        <v>16</v>
+      <c r="L8">
+        <f>D8+E8+F8+G8+H8+I8+J8+K8</f>
+        <v>34</v>
       </c>
       <c r="M8">
-        <f>D8+E8+F8+G8+H8+I8+J8+K8</f>
-        <v>32</v>
-      </c>
-      <c r="N8">
-        <f>M8*3</f>
-        <v>96</v>
-      </c>
-      <c r="O8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+        <f>L8*3</f>
+        <v>102</v>
+      </c>
+      <c r="N8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
         <v>7</v>
       </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="L9">
         <f>D9+E9+F9+G9+H9+I9+J9+K9</f>
         <v>34</v>
       </c>
-      <c r="N9">
-        <f>M9*3</f>
+      <c r="M9">
+        <f>L9*3</f>
         <v>102</v>
       </c>
-      <c r="O9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I10">
         <v>3</v>
       </c>
       <c r="J10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
-      <c r="L10" t="s">
-        <v>16</v>
+      <c r="L10">
+        <f>D10+E10+F10+G10+H10+I10+J10+K10</f>
+        <v>32</v>
       </c>
       <c r="M10">
-        <f>D10+E10+F10+G10+H10+I10+J10+K10</f>
-        <v>35</v>
-      </c>
-      <c r="N10">
-        <f>M10*3</f>
-        <v>105</v>
-      </c>
-      <c r="O10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+        <f>L10*3</f>
+        <v>96</v>
+      </c>
+      <c r="N10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -1023,45 +1199,42 @@
       <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11">
+      <c r="L11">
         <f>D11+E11+F11+G11+H11+I11+J11+K11</f>
         <v>34</v>
       </c>
-      <c r="N11">
-        <f>M11*3</f>
+      <c r="M11">
+        <f>L11*3</f>
         <v>102</v>
       </c>
-      <c r="O11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
         <v>8</v>
-      </c>
-      <c r="H12">
-        <v>7</v>
       </c>
       <c r="I12">
         <v>3</v>
@@ -1072,39 +1245,36 @@
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="L12" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12">
+      <c r="L12">
         <f>D12+E12+F12+G12+H12+I12+J12+K12</f>
         <v>34</v>
       </c>
-      <c r="N12">
-        <f>M12*3</f>
+      <c r="M12">
+        <f>L12*3</f>
         <v>102</v>
       </c>
-      <c r="O12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -1121,45 +1291,42 @@
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13" t="s">
-        <v>16</v>
+      <c r="L13">
+        <f>D13+E13+F13+G13+H13+I13+J13+K13</f>
+        <v>32</v>
       </c>
       <c r="M13">
-        <f>D13+E13+F13+G13+H13+I13+J13+K13</f>
-        <v>34</v>
-      </c>
-      <c r="N13">
-        <f>M13*3</f>
-        <v>102</v>
-      </c>
-      <c r="O13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+        <f>L13*3</f>
+        <v>96</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
       <c r="H14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I14">
         <v>3</v>
@@ -1170,76 +1337,284 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14" t="s">
-        <v>16</v>
+      <c r="L14">
+        <f>D14+E14+F14+G14+H14+I14+J14+K14</f>
+        <v>33</v>
       </c>
       <c r="M14">
-        <f>D14+E14+F14+G14+H14+I14+J14+K14</f>
-        <v>32</v>
-      </c>
-      <c r="N14">
-        <f>M14*3</f>
-        <v>96</v>
-      </c>
-      <c r="O14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+        <f>L14*3</f>
+        <v>99</v>
+      </c>
+      <c r="N14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <v>7</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15">
         <v>3</v>
       </c>
       <c r="H15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <f>D15+E15+F15+G15+H15+I15+J15+K15</f>
+        <v>34</v>
       </c>
       <c r="M15">
-        <f>D15+E15+F15+G15+H15+I15+J15+K15</f>
-        <v>33</v>
-      </c>
-      <c r="N15">
-        <f>M15*3</f>
-        <v>99</v>
-      </c>
-      <c r="O15" t="s">
-        <v>45</v>
+        <f>L15*3</f>
+        <v>102</v>
+      </c>
+      <c r="N15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:O3" xr:uid="{F63DEB86-B494-49C7-AE29-DB56967CB25B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:O15">
-      <sortCondition ref="A3"/>
+  <autoFilter ref="A3:N3" xr:uid="{F63DEB86-B494-49C7-AE29-DB56967CB25B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N15">
+      <sortCondition ref="E3"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF86FB7-6CD0-44E0-BFBD-0DCA846E71AC}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="46" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="46" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="46" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="46" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:G3" xr:uid="{9CF86FB7-6CD0-44E0-BFBD-0DCA846E71AC}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v2.1.4 update: Reworked armour system - New armour system - uses the five damage types. - Updated Faction / Leadership Selectin - now a clear process to follow. - Added maximum selections for all units to 1.
</commit_message>
<xml_diff>
--- a/metrics/XCOM Enemy Eternal - Costs and Statistics.xlsx
+++ b/metrics/XCOM Enemy Eternal - Costs and Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phoenix\source\repos\Eklipse-Games\xcom-enemyeternal\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0AC23A-262C-4423-AB3C-0EF13AD26E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0081D32-99BA-4083-9303-23425783546A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EB47B550-E58A-4646-B89E-9CBA77073B0E}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'AI STATS'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UNIT STATS'!$A$3:$N$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UNIT STATS'!$A$3:$O$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'WEAPON STATS'!$A$3:$N$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="138">
   <si>
     <t>AIM</t>
   </si>
@@ -569,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -586,25 +586,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63DEB86-B494-49C7-AE29-DB56967CB25B}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -955,799 +950,849 @@
     <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="9"/>
+      <c r="L3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="10">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10">
+        <v>7</v>
+      </c>
+      <c r="F4" s="10">
+        <v>4</v>
+      </c>
+      <c r="G4" s="10">
+        <v>3</v>
+      </c>
+      <c r="H4" s="10">
+        <v>10</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="L4" s="7">
+        <v>3</v>
+      </c>
+      <c r="M4" s="10">
+        <f>D4+E4+F4+G4+H4+I4+J4+L4</f>
+        <v>34</v>
+      </c>
+      <c r="N4" s="10">
+        <f>M4*3</f>
+        <v>102</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="10">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10">
+        <v>5</v>
+      </c>
+      <c r="G5" s="10">
+        <v>7</v>
+      </c>
+      <c r="H5" s="10">
+        <v>9</v>
+      </c>
+      <c r="I5" s="10">
+        <v>3</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="7">
+        <v>2</v>
+      </c>
+      <c r="M5" s="10">
+        <f>D5+E5+F5+G5+H5+I5+J5+L5</f>
+        <v>35</v>
+      </c>
+      <c r="N5" s="10">
+        <f>M5*3</f>
+        <v>105</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="10">
+        <v>7</v>
+      </c>
+      <c r="E6" s="10">
+        <v>5</v>
+      </c>
+      <c r="F6" s="10">
+        <v>5</v>
+      </c>
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="H6" s="10">
+        <v>9</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6" s="10">
+        <f>D6+E6+F6+G6+H6+I6+J6+L6</f>
+        <v>33</v>
+      </c>
+      <c r="N6" s="10">
+        <f>M6*3</f>
+        <v>99</v>
+      </c>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10">
+        <v>5</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10">
+        <v>3</v>
+      </c>
+      <c r="H7" s="10">
+        <v>7</v>
+      </c>
+      <c r="I7" s="10">
+        <v>3</v>
+      </c>
+      <c r="J7" s="10">
+        <v>8</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="10">
+        <f>D7+E7+F7+G7+H7+I7+J7+L7</f>
+        <v>35</v>
+      </c>
+      <c r="N7" s="10">
+        <f>M7*3</f>
+        <v>105</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="10">
+        <v>6</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6</v>
+      </c>
+      <c r="G8" s="10">
+        <v>7</v>
+      </c>
+      <c r="H8" s="10">
+        <v>8</v>
+      </c>
+      <c r="I8" s="10">
+        <v>3</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="10">
+        <f>D8+E8+F8+G8+H8+I8+J8+L8</f>
+        <v>34</v>
+      </c>
+      <c r="N8" s="10">
+        <f>M8*3</f>
+        <v>102</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="10">
+        <v>8</v>
+      </c>
+      <c r="E9" s="10">
+        <v>4</v>
+      </c>
+      <c r="F9" s="10">
+        <v>7</v>
+      </c>
+      <c r="G9" s="10">
+        <v>3</v>
+      </c>
+      <c r="H9" s="10">
+        <v>8</v>
+      </c>
+      <c r="I9" s="10">
+        <v>3</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="10">
+        <f>D9+E9+F9+G9+H9+I9+J9+L9</f>
+        <v>34</v>
+      </c>
+      <c r="N9" s="10">
+        <f>M9*3</f>
+        <v>102</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="10">
+        <v>7</v>
+      </c>
+      <c r="E10" s="10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10">
+        <v>6</v>
+      </c>
+      <c r="G10" s="10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="10">
+        <v>8</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="7">
+        <v>1</v>
+      </c>
+      <c r="M10" s="10">
+        <f>D10+E10+F10+G10+H10+I10+J10+L10</f>
+        <v>32</v>
+      </c>
+      <c r="N10" s="10">
+        <f>M10*3</f>
+        <v>96</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="10">
+        <v>8</v>
+      </c>
+      <c r="E11" s="10">
+        <v>3</v>
+      </c>
+      <c r="F11" s="10">
+        <v>6</v>
+      </c>
+      <c r="G11" s="10">
+        <v>4</v>
+      </c>
+      <c r="H11" s="10">
+        <v>7</v>
+      </c>
+      <c r="I11" s="10">
+        <v>6</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
+        <f>D11+E11+F11+G11+H11+I11+J11+L11</f>
+        <v>34</v>
+      </c>
+      <c r="N11" s="10">
+        <f>M11*3</f>
+        <v>102</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B12" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="10">
+        <v>5</v>
+      </c>
+      <c r="E12" s="10">
+        <v>6</v>
+      </c>
+      <c r="F12" s="10">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10">
+        <v>6</v>
+      </c>
+      <c r="H12" s="10">
+        <v>10</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L12" s="7">
+        <v>3</v>
+      </c>
+      <c r="M12" s="10">
+        <f>D12+E12+F12+G12+H12+I12+J12+L12</f>
+        <v>34</v>
+      </c>
+      <c r="N12" s="10">
+        <f>M12*3</f>
+        <v>102</v>
+      </c>
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D13" s="10">
         <v>7</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E13" s="10">
         <v>5</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F13" s="10">
         <v>5</v>
       </c>
-      <c r="G4" s="7">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="G13" s="10">
+        <v>3</v>
+      </c>
+      <c r="H13" s="10">
         <v>9</v>
       </c>
-      <c r="I4" s="7">
-        <v>3</v>
-      </c>
-      <c r="J4" s="7">
+      <c r="I13" s="10">
+        <v>3</v>
+      </c>
+      <c r="J13" s="10">
         <v>0</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K13" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L13" s="7">
         <v>1</v>
       </c>
-      <c r="L4" s="7">
-        <f t="shared" ref="L4:L19" si="0">D4+E4+F4+G4+H4+I4+J4+K4</f>
+      <c r="M13" s="10">
+        <f>D13+E13+F13+G13+H13+I13+J13+L13</f>
         <v>33</v>
       </c>
-      <c r="M4" s="7">
-        <f t="shared" ref="M4:M19" si="1">L4*3</f>
+      <c r="N13" s="10">
+        <f>M13*3</f>
         <v>99</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O13" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="10">
+        <v>5</v>
+      </c>
+      <c r="E14" s="10">
+        <v>3</v>
+      </c>
+      <c r="F14" s="10">
+        <v>5</v>
+      </c>
+      <c r="G14" s="10">
+        <v>3</v>
+      </c>
+      <c r="H14" s="10">
+        <v>7</v>
+      </c>
+      <c r="I14" s="10">
+        <v>3</v>
+      </c>
+      <c r="J14" s="10">
+        <v>8</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1</v>
+      </c>
+      <c r="M14" s="10">
+        <f>D14+E14+F14+G14+H14+I14+J14+L14</f>
+        <v>35</v>
+      </c>
+      <c r="N14" s="10">
+        <f>M14*3</f>
+        <v>105</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="10">
+        <v>9</v>
+      </c>
+      <c r="E15" s="10">
+        <v>4</v>
+      </c>
+      <c r="F15" s="10">
+        <v>6</v>
+      </c>
+      <c r="G15" s="10">
+        <v>4</v>
+      </c>
+      <c r="H15" s="10">
+        <v>7</v>
+      </c>
+      <c r="I15" s="10">
+        <v>3</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="10">
+        <f>D15+E15+F15+G15+H15+I15+J15+L15</f>
+        <v>34</v>
+      </c>
+      <c r="N15" s="10">
+        <f>M15*3</f>
         <v>102</v>
       </c>
-      <c r="D5" s="7">
+      <c r="O15" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="10">
+        <v>6</v>
+      </c>
+      <c r="E16" s="10">
+        <v>3</v>
+      </c>
+      <c r="F16" s="10">
+        <v>6</v>
+      </c>
+      <c r="G16" s="10">
+        <v>8</v>
+      </c>
+      <c r="H16" s="10">
         <v>7</v>
       </c>
-      <c r="E5" s="7">
+      <c r="I16" s="10">
+        <v>3</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
+      <c r="M16" s="10">
+        <f>D16+E16+F16+G16+H16+I16+J16+L16</f>
+        <v>34</v>
+      </c>
+      <c r="N16" s="10">
+        <f>M16*3</f>
+        <v>102</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="10">
+        <v>7</v>
+      </c>
+      <c r="E17" s="10">
+        <v>4</v>
+      </c>
+      <c r="F17" s="10">
         <v>5</v>
       </c>
-      <c r="F5" s="7">
-        <v>5</v>
-      </c>
-      <c r="G5" s="7">
-        <v>3</v>
-      </c>
-      <c r="H5" s="7">
+      <c r="G17" s="10">
+        <v>6</v>
+      </c>
+      <c r="H17" s="10">
         <v>9</v>
       </c>
-      <c r="I5" s="7">
-        <v>3</v>
-      </c>
-      <c r="J5" s="7">
+      <c r="I17" s="10">
+        <v>3</v>
+      </c>
+      <c r="J17" s="10">
         <v>0</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K17" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L17" s="7">
         <v>1</v>
       </c>
-      <c r="L5" s="7">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="M5" s="7">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="M17" s="10">
+        <f>D17+E17+F17+G17+H17+I17+J17+L17</f>
+        <v>35</v>
+      </c>
+      <c r="N17" s="10">
+        <f>M17*3</f>
+        <v>105</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="10">
+        <v>8</v>
+      </c>
+      <c r="E18" s="10">
+        <v>4</v>
+      </c>
+      <c r="F18" s="10">
         <v>7</v>
       </c>
-      <c r="E6" s="7">
+      <c r="G18" s="10">
+        <v>3</v>
+      </c>
+      <c r="H18" s="10">
+        <v>8</v>
+      </c>
+      <c r="I18" s="10">
+        <v>3</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="7">
+        <v>1</v>
+      </c>
+      <c r="M18" s="10">
+        <f>D18+E18+F18+G18+H18+I18+J18+L18</f>
+        <v>34</v>
+      </c>
+      <c r="N18" s="10">
+        <f>M18*3</f>
+        <v>102</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="10">
         <v>7</v>
       </c>
-      <c r="F6" s="7">
+      <c r="E19" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="7">
-        <v>3</v>
-      </c>
-      <c r="H6" s="7">
-        <v>10</v>
-      </c>
-      <c r="I6" s="7">
+      <c r="F19" s="10">
+        <v>6</v>
+      </c>
+      <c r="G19" s="10">
+        <v>3</v>
+      </c>
+      <c r="H19" s="10">
+        <v>8</v>
+      </c>
+      <c r="I19" s="10">
+        <v>3</v>
+      </c>
+      <c r="J19" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
-        <v>3</v>
-      </c>
-      <c r="L6" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M6" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="7">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7">
-        <v>6</v>
-      </c>
-      <c r="F7" s="7">
-        <v>4</v>
-      </c>
-      <c r="G7" s="7">
-        <v>6</v>
-      </c>
-      <c r="H7" s="7">
-        <v>10</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>3</v>
-      </c>
-      <c r="L7" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M7" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="7">
-        <v>5</v>
-      </c>
-      <c r="E8" s="7">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7">
-        <v>5</v>
-      </c>
-      <c r="G8" s="7">
-        <v>3</v>
-      </c>
-      <c r="H8" s="7">
-        <v>7</v>
-      </c>
-      <c r="I8" s="7">
-        <v>3</v>
-      </c>
-      <c r="J8" s="7">
-        <v>8</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="K19" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L19" s="7">
         <v>1</v>
       </c>
-      <c r="L8" s="7">
-        <f t="shared" si="0"/>
+      <c r="M19" s="10">
+        <f>D19+E19+F19+G19+H19+I19+J19+L19</f>
+        <v>32</v>
+      </c>
+      <c r="N19" s="10">
+        <f>M19*3</f>
+        <v>96</v>
+      </c>
+      <c r="O19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="7">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="7">
-        <v>5</v>
-      </c>
-      <c r="E9" s="7">
-        <v>3</v>
-      </c>
-      <c r="F9" s="7">
-        <v>5</v>
-      </c>
-      <c r="G9" s="7">
-        <v>3</v>
-      </c>
-      <c r="H9" s="7">
-        <v>7</v>
-      </c>
-      <c r="I9" s="7">
-        <v>3</v>
-      </c>
-      <c r="J9" s="7">
-        <v>8</v>
-      </c>
-      <c r="K9" s="7">
-        <v>1</v>
-      </c>
-      <c r="L9" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M9" s="7">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="7">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7">
-        <v>3</v>
-      </c>
-      <c r="F10" s="7">
-        <v>6</v>
-      </c>
-      <c r="G10" s="7">
-        <v>4</v>
-      </c>
-      <c r="H10" s="7">
-        <v>7</v>
-      </c>
-      <c r="I10" s="7">
-        <v>6</v>
-      </c>
-      <c r="J10" s="7">
-        <v>0</v>
-      </c>
-      <c r="K10" s="7">
-        <v>0</v>
-      </c>
-      <c r="L10" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M10" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="7">
-        <v>9</v>
-      </c>
-      <c r="E11" s="7">
-        <v>4</v>
-      </c>
-      <c r="F11" s="7">
-        <v>6</v>
-      </c>
-      <c r="G11" s="7">
-        <v>4</v>
-      </c>
-      <c r="H11" s="7">
-        <v>7</v>
-      </c>
-      <c r="I11" s="7">
-        <v>3</v>
-      </c>
-      <c r="J11" s="7">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7">
-        <v>1</v>
-      </c>
-      <c r="L11" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M11" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="7">
-        <v>6</v>
-      </c>
-      <c r="E12" s="7">
-        <v>3</v>
-      </c>
-      <c r="F12" s="7">
-        <v>6</v>
-      </c>
-      <c r="G12" s="7">
-        <v>7</v>
-      </c>
-      <c r="H12" s="7">
-        <v>8</v>
-      </c>
-      <c r="I12" s="7">
-        <v>3</v>
-      </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
-      <c r="K12" s="7">
-        <v>1</v>
-      </c>
-      <c r="L12" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M12" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="7">
-        <v>6</v>
-      </c>
-      <c r="E13" s="7">
-        <v>3</v>
-      </c>
-      <c r="F13" s="7">
-        <v>6</v>
-      </c>
-      <c r="G13" s="7">
-        <v>8</v>
-      </c>
-      <c r="H13" s="7">
-        <v>7</v>
-      </c>
-      <c r="I13" s="7">
-        <v>3</v>
-      </c>
-      <c r="J13" s="7">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7">
-        <v>1</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M13" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="7">
-        <v>7</v>
-      </c>
-      <c r="E14" s="7">
-        <v>4</v>
-      </c>
-      <c r="F14" s="7">
-        <v>5</v>
-      </c>
-      <c r="G14" s="7">
-        <v>6</v>
-      </c>
-      <c r="H14" s="7">
-        <v>9</v>
-      </c>
-      <c r="I14" s="7">
-        <v>3</v>
-      </c>
-      <c r="J14" s="7">
-        <v>0</v>
-      </c>
-      <c r="K14" s="7">
-        <v>1</v>
-      </c>
-      <c r="L14" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M14" s="7">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="7">
-        <v>6</v>
-      </c>
-      <c r="E15" s="7">
-        <v>3</v>
-      </c>
-      <c r="F15" s="7">
-        <v>5</v>
-      </c>
-      <c r="G15" s="7">
-        <v>7</v>
-      </c>
-      <c r="H15" s="7">
-        <v>9</v>
-      </c>
-      <c r="I15" s="7">
-        <v>3</v>
-      </c>
-      <c r="J15" s="7">
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="7">
-        <v>8</v>
-      </c>
-      <c r="E16" s="7">
-        <v>4</v>
-      </c>
-      <c r="F16" s="7">
-        <v>7</v>
-      </c>
-      <c r="G16" s="7">
-        <v>3</v>
-      </c>
-      <c r="H16" s="7">
-        <v>8</v>
-      </c>
-      <c r="I16" s="7">
-        <v>3</v>
-      </c>
-      <c r="J16" s="7">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7">
-        <v>1</v>
-      </c>
-      <c r="L16" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M16" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="7">
-        <v>8</v>
-      </c>
-      <c r="E17" s="7">
-        <v>4</v>
-      </c>
-      <c r="F17" s="7">
-        <v>7</v>
-      </c>
-      <c r="G17" s="7">
-        <v>3</v>
-      </c>
-      <c r="H17" s="7">
-        <v>8</v>
-      </c>
-      <c r="I17" s="7">
-        <v>3</v>
-      </c>
-      <c r="J17" s="7">
-        <v>0</v>
-      </c>
-      <c r="K17" s="7">
-        <v>1</v>
-      </c>
-      <c r="L17" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M17" s="7">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="7">
-        <v>7</v>
-      </c>
-      <c r="E18" s="7">
-        <v>4</v>
-      </c>
-      <c r="F18" s="7">
-        <v>6</v>
-      </c>
-      <c r="G18" s="7">
-        <v>3</v>
-      </c>
-      <c r="H18" s="7">
-        <v>8</v>
-      </c>
-      <c r="I18" s="7">
-        <v>3</v>
-      </c>
-      <c r="J18" s="7">
-        <v>0</v>
-      </c>
-      <c r="K18" s="7">
-        <v>1</v>
-      </c>
-      <c r="L18" s="7">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="M18" s="7">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="7">
-        <v>7</v>
-      </c>
-      <c r="E19" s="7">
-        <v>4</v>
-      </c>
-      <c r="F19" s="7">
-        <v>6</v>
-      </c>
-      <c r="G19" s="7">
-        <v>3</v>
-      </c>
-      <c r="H19" s="7">
-        <v>8</v>
-      </c>
-      <c r="I19" s="7">
-        <v>3</v>
-      </c>
-      <c r="J19" s="7">
-        <v>0</v>
-      </c>
-      <c r="K19" s="7">
-        <v>1</v>
-      </c>
-      <c r="L19" s="7">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="M19" s="7">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>35</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:N3" xr:uid="{F63DEB86-B494-49C7-AE29-DB56967CB25B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N19">
-      <sortCondition ref="B3"/>
+  <autoFilter ref="A3:O3" xr:uid="{F63DEB86-B494-49C7-AE29-DB56967CB25B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:O19">
+      <sortCondition ref="A3"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1973,14 +2018,14 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.08984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" style="5" bestFit="1" customWidth="1"/>
@@ -2001,591 +2046,591 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="7">
         <v>18</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="7">
         <v>36</v>
       </c>
-      <c r="D4" s="13">
-        <v>3</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="8">
         <v>4</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="8">
         <v>5</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="9">
-        <f>C4+(D4*5)</f>
+      <c r="L4" s="7">
+        <f t="shared" ref="L4:L11" si="0">C4+(D4*5)</f>
         <v>51</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="7">
         <f>C4+(H4*5)</f>
         <v>56</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="7">
         <f>C4+(J4*5)</f>
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="7">
         <v>18</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="7">
         <v>36</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L5" s="9">
-        <f>C5+(D5*5)</f>
+      <c r="H5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="M5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="7">
         <v>15</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="7">
         <v>30</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="8">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="8">
         <v>6</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="8">
         <v>8</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L6" s="9">
-        <f>C6+(D6*5)</f>
+      <c r="L6" s="7">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="M6" s="9">
-        <f>C6+(H6*5)</f>
+      <c r="M6" s="7">
+        <f t="shared" ref="M6:M11" si="1">C6+(H6*5)</f>
         <v>60</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="7">
         <f>C6+(J6*5)</f>
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="7">
         <v>15</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="7">
         <v>30</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="H7" s="13">
-        <v>3</v>
-      </c>
-      <c r="I7" s="9" t="s">
+      <c r="H7" s="8">
+        <v>3</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="8">
         <v>4</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="L7" s="9">
-        <f>C7+(D7*5)</f>
+      <c r="L7" s="7">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="M7" s="9">
-        <f>C7+(H7*5)</f>
+      <c r="M7" s="7">
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="7">
         <f>C7+(J7*5)</f>
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="7">
         <v>15</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="7">
         <v>30</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="8">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="8">
         <v>10</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J8" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L8" s="9">
-        <f>C8+(D8*5)</f>
+      <c r="J8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="M8" s="9">
-        <f>C8+(H8*5)</f>
+      <c r="M8" s="7">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="7">
         <v>12</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="7">
         <v>24</v>
       </c>
-      <c r="D9" s="13">
-        <v>3</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="8">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" s="13">
+      <c r="F9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="8">
         <v>4</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="8">
         <v>5</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L9" s="9">
-        <f>C9+(D9*5)</f>
+      <c r="L9" s="7">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="M9" s="9">
-        <f>C9+(H9*5)</f>
+      <c r="M9" s="7">
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="7">
         <f>C9+(J9*5)</f>
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="7">
         <v>9</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="7">
         <v>18</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="8">
         <v>4</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H10" s="13">
+      <c r="F10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="8">
         <v>5</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="8">
         <v>6</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L10" s="9">
-        <f>C10+(D10*5)</f>
+      <c r="L10" s="7">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="M10" s="9">
-        <f>C10+(H10*5)</f>
+      <c r="M10" s="7">
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="7">
         <f>C10+(J10*5)</f>
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="7">
         <v>9</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="7">
         <v>18</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="8">
         <v>2</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H11" s="13">
-        <v>3</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="F11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="8">
         <v>4</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L11" s="9">
-        <f>C11+(D11*5)</f>
+      <c r="L11" s="7">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="M11" s="9">
-        <f>C11+(H11*5)</f>
+      <c r="M11" s="7">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="7">
         <f>C11+(J11*5)</f>
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="7">
         <v>0</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="7">
         <v>0</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="8">
         <v>8</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L12" s="9">
+      <c r="F12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" s="7">
         <f>D12*10</f>
         <v>80</v>
       </c>
-      <c r="M12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="N12" s="9" t="s">
+      <c r="M12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="7">
         <v>0</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="7">
         <v>0</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L13" s="9">
+      <c r="D13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L13" s="7">
         <v>25</v>
       </c>
-      <c r="M13" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="N13" s="9" t="s">
+      <c r="M13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N13" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="7">
         <v>0</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="7">
         <v>0</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="8">
         <v>5</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G14" s="9" t="s">
+      <c r="F14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L14" s="9">
+      <c r="H14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L14" s="7">
         <f>D14*10</f>
         <v>50</v>
       </c>
-      <c r="M14" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="N14" s="9" t="s">
+      <c r="M14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N14" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="7">
         <v>0</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="7">
         <v>0</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="8">
         <v>4</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="13">
+      <c r="F15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="8">
         <v>5</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="8">
         <v>6</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="7">
         <f>D15*10</f>
         <v>40</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="7">
         <f>H15*10</f>
         <v>50</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="7">
         <f>J15*10</f>
         <v>60</v>
       </c>

</xml_diff>